<commit_message>
Updated section about experments
Added more charts
</commit_message>
<xml_diff>
--- a/report/Metrics.xlsx
+++ b/report/Metrics.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>Main</t>
   </si>
@@ -105,9 +105,6 @@
     <t>2m</t>
   </si>
   <si>
-    <t>Median% =</t>
-  </si>
-  <si>
     <t>Median</t>
   </si>
   <si>
@@ -131,6 +128,18 @@
   <si>
     <t>Failed to sent</t>
   </si>
+  <si>
+    <t>Helper #1</t>
+  </si>
+  <si>
+    <t>Helper #2</t>
+  </si>
+  <si>
+    <t>Helper #3</t>
+  </si>
+  <si>
+    <t>Helper #4</t>
+  </si>
 </sst>
 </file>
 
@@ -148,22 +157,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -182,23 +198,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -328,16 +484,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>809</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>835</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>809</c:v>
-                </c:pt>
                 <c:pt idx="2">
+                  <c:v>994</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1207</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -374,16 +530,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>1570</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1616</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>1570</c:v>
-                </c:pt>
                 <c:pt idx="2">
+                  <c:v>1843</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2345</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1843</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,16 +576,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>35</c:v>
-                </c:pt>
                 <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -445,11 +601,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="313761048"/>
-        <c:axId val="313784592"/>
+        <c:axId val="108784936"/>
+        <c:axId val="108785328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="313761048"/>
+        <c:axId val="108784936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -491,7 +647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313784592"/>
+        <c:crossAx val="108785328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -499,7 +655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="313784592"/>
+        <c:axId val="108785328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -550,7 +706,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313761048"/>
+        <c:crossAx val="108784936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -874,7 +1030,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$35:$B$37</c:f>
+              <c:f>Sheet1!$B$34:$B$36</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -891,18 +1047,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$35:$C$37</c:f>
+              <c:f>Sheet1!$C$34:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>914.5</c:v>
+                  <c:v>822</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1729.5</c:v>
+                  <c:v>1593</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1230,7 +1386,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$64:$B$66</c:f>
+              <c:f>Sheet1!$B$63:$B$65</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1247,7 +1403,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$64:$C$66</c:f>
+              <c:f>Sheet1!$C$63:$C$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1744,11 +1900,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="314089024"/>
-        <c:axId val="313230248"/>
+        <c:axId val="268586880"/>
+        <c:axId val="268590800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="314089024"/>
+        <c:axId val="268586880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1790,7 +1946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313230248"/>
+        <c:crossAx val="268590800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1798,7 +1954,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="313230248"/>
+        <c:axId val="268590800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1849,7 +2005,800 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314089024"/>
+        <c:crossAx val="268586880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$77</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Helper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$78:$C$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$77</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Clients</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$78:$D$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="95160056"/>
+        <c:axId val="95156920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="95160056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95156920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="95156920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95160056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Client</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Helper Distribution</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$91</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Helper #1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$92:$C$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$91</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Helper #2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$92:$D$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$91</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Helper #3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$92:$E$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$91</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Helper #4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$92:$F$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="333619992"/>
+        <c:axId val="269973784"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="333619992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="269973784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="269973784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333619992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2090,6 +3039,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3530,6 +4559,1012 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4038,13 +6073,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4068,13 +6103,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>109537</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>452437</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4098,13 +6133,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>157162</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>500062</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4134,7 +6169,7 @@
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4154,12 +6189,75 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A24:I31" totalsRowShown="0">
-  <autoFilter ref="A24:I31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A24:I30" totalsRowShown="0">
+  <autoFilter ref="A24:I30"/>
+  <sortState ref="A25:J31">
+    <sortCondition ref="C24:C31"/>
+  </sortState>
   <tableColumns count="9">
     <tableColumn id="1" name="Main"/>
     <tableColumn id="2" name="Total messages sent"/>
@@ -4178,11 +6276,11 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A10:N22" totalsRowShown="0">
   <autoFilter ref="A10:N22"/>
-  <sortState ref="A11:N22">
-    <sortCondition ref="E10:E22"/>
+  <sortState ref="A11:O22">
+    <sortCondition ref="F10:F22"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Main" dataDxfId="0"/>
+    <tableColumn id="1" name="Main" dataDxfId="6"/>
     <tableColumn id="2" name="Helper"/>
     <tableColumn id="3" name="Clients"/>
     <tableColumn id="4" name="Clients end"/>
@@ -4196,6 +6294,38 @@
     <tableColumn id="11" name="F Received"/>
     <tableColumn id="12" name="Changerequest"/>
     <tableColumn id="13" name="Run time"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B77:D87" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="5">
+  <autoFilter ref="B77:D87"/>
+  <sortState ref="C78:E87">
+    <sortCondition ref="C77:C87"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Main" dataDxfId="4"/>
+    <tableColumn id="2" name="Helper" dataDxfId="3"/>
+    <tableColumn id="3" name="Clients" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B91:F94" totalsRowShown="0">
+  <autoFilter ref="B91:F94"/>
+  <sortState ref="B92:F94">
+    <sortCondition ref="B91:B94"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="5" name="Helper"/>
+    <tableColumn id="1" name="Helper #1"/>
+    <tableColumn id="2" name="Helper #2"/>
+    <tableColumn id="3" name="Helper #3"/>
+    <tableColumn id="4" name="Helper #4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4464,15 +6594,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A10:N66"/>
+  <dimension ref="A10:N94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P54" sqref="P54"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
@@ -4499,19 +6630,19 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
         <v>28</v>
       </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>31</v>
-      </c>
-      <c r="H10" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" t="s">
-        <v>32</v>
       </c>
       <c r="J10" t="s">
         <v>14</v>
@@ -4792,7 +6923,7 @@
       <c r="M19">
         <v>0</v>
       </c>
-      <c r="N19" s="4" t="s">
+      <c r="N19" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4833,7 +6964,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E22">
         <f xml:space="preserve"> MEDIAN(E6:E12)</f>
@@ -4861,13 +6992,13 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
         <v>28</v>
       </c>
-      <c r="C24" t="s">
-        <v>29</v>
-      </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
         <v>3</v>
@@ -4887,16 +7018,16 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25">
-        <v>835</v>
+        <v>809</v>
       </c>
       <c r="C25">
-        <v>1616</v>
+        <v>1570</v>
       </c>
       <c r="D25">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -4911,21 +7042,21 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26">
-        <v>809</v>
+        <v>835</v>
       </c>
       <c r="C26">
-        <v>1570</v>
+        <v>1616</v>
       </c>
       <c r="D26">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4940,21 +7071,21 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>1207</v>
+        <v>994</v>
       </c>
       <c r="C27">
-        <v>2345</v>
+        <v>1843</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4969,28 +7100,21 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>10</v>
-      </c>
-      <c r="K27" t="s">
-        <v>26</v>
-      </c>
-      <c r="L27" s="2">
-        <f xml:space="preserve"> (D31/C31)</f>
-        <v>1.2720439433362244E-2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28">
-        <v>994</v>
+        <v>1207</v>
       </c>
       <c r="C28">
-        <v>1843</v>
+        <v>2345</v>
       </c>
       <c r="D28">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -5005,113 +7129,271 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31">
-        <f>MEDIAN(B25:B30)</f>
-        <v>914.5</v>
-      </c>
-      <c r="C31">
-        <f t="shared" ref="C31:H31" si="0">MEDIAN(C25:C30)</f>
-        <v>1729.5</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <f>MEDIAN(B21:B26)</f>
+        <v>822</v>
+      </c>
+      <c r="C30">
+        <f>MEDIAN(C21:C26)</f>
+        <v>1593</v>
+      </c>
+      <c r="D30">
+        <f>MEDIAN(D21:D26)</f>
+        <v>28.5</v>
+      </c>
+      <c r="E30">
+        <f>MEDIAN(E21:E26)</f>
         <v>0</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="0"/>
+      <c r="F30">
+        <f>MEDIAN(F21:F26)</f>
         <v>0</v>
       </c>
-      <c r="G31">
-        <f t="shared" si="0"/>
+      <c r="G30">
+        <f>MEDIAN(G21:G26)</f>
         <v>0</v>
       </c>
-      <c r="H31">
-        <f t="shared" si="0"/>
+      <c r="H30">
+        <f>MEDIAN(H21:H26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>0</v>
+      <c r="B34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <f>B30</f>
+        <v>822</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
-        <v>1</v>
+      <c r="B35" t="s">
+        <v>2</v>
       </c>
       <c r="C35">
-        <f>B31</f>
-        <v>914.5</v>
+        <f xml:space="preserve"> C30</f>
+        <v>1593</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C36">
-        <f>C31</f>
-        <v>1729.5</v>
+        <f>D30</f>
+        <v>28.5</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37">
-        <f>D31</f>
-        <v>22</v>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <f xml:space="preserve"> E22</f>
+        <v>389</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C64">
-        <f xml:space="preserve"> E22</f>
-        <v>389</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>2</v>
-      </c>
-      <c r="C65">
         <f>H22</f>
         <v>453.5</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>34</v>
-      </c>
-      <c r="C66">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65">
         <f>I22</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4">
+        <v>1</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1</v>
+      </c>
+      <c r="D78" s="4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="4">
+        <v>1</v>
+      </c>
+      <c r="C79" s="4">
+        <v>2</v>
+      </c>
+      <c r="D79" s="4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="4">
+        <v>2</v>
+      </c>
+      <c r="C80" s="4">
+        <v>1</v>
+      </c>
+      <c r="D80" s="4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="4">
+        <v>2</v>
+      </c>
+      <c r="C81" s="4">
+        <v>2</v>
+      </c>
+      <c r="D81" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="4">
+        <v>2</v>
+      </c>
+      <c r="C82" s="4">
+        <v>3</v>
+      </c>
+      <c r="D82" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" s="4">
+        <v>2</v>
+      </c>
+      <c r="C83" s="4">
+        <v>4</v>
+      </c>
+      <c r="D83" s="4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="4">
+        <v>3</v>
+      </c>
+      <c r="C84" s="4">
+        <v>1</v>
+      </c>
+      <c r="D84" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" s="5"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C91" t="s">
+        <v>34</v>
+      </c>
+      <c r="D91" t="s">
+        <v>35</v>
+      </c>
+      <c r="E91" t="s">
+        <v>36</v>
+      </c>
+      <c r="F91" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>41</v>
+      </c>
+      <c r="D92">
+        <v>26</v>
+      </c>
+      <c r="E92">
+        <v>30</v>
+      </c>
+      <c r="F92">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>2</v>
+      </c>
+      <c r="C93">
+        <v>56</v>
+      </c>
+      <c r="D93">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>3</v>
+      </c>
+      <c r="C94">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="4">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Improved background on application
</commit_message>
<xml_diff>
--- a/report/Metrics.xlsx
+++ b/report/Metrics.xlsx
@@ -6163,14 +6163,14 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6596,8 +6596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A10:N94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="I7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI29" sqref="AI29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>